<commit_message>
Houston climb 10 for 10
Signed-off-by: Omar Vargas <ovswscrum@gmail.com>
</commit_message>
<xml_diff>
--- a/src/other/TestRun.xlsx
+++ b/src/other/TestRun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FRC2019\projects\FRC_2019\src\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E817E22E-19C0-4BC1-B72D-C8E425C270DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743D000F-151B-4D1A-ABDD-C0DE589FF143}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="15820" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36238,8 +36238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D413"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:D197"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:D144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>